<commit_message>
q_h and q_t and n0 bugs fixed
</commit_message>
<xml_diff>
--- a/Exchange Rate/test.xlsx
+++ b/Exchange Rate/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>YYYY/MM/DD</t>
   </si>
@@ -37,15 +37,6 @@
   </si>
   <si>
     <t>0.84932</t>
-  </si>
-  <si>
-    <t>0.84624</t>
-  </si>
-  <si>
-    <t>0.84997</t>
-  </si>
-  <si>
-    <t>0.84789</t>
   </si>
 </sst>
 </file>
@@ -874,7 +865,7 @@
   <dimension ref="A1:B146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -923,36 +914,16 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>43258</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>43259</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>43262</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>43263</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1"/>

</xml_diff>